<commit_message>
Adicionado quantidade de horas por caso de uso
</commit_message>
<xml_diff>
--- a/Docs/Entrega do dia 21-11/backlog_inicial.xlsx
+++ b/Docs/Entrega do dia 21-11/backlog_inicial.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,9 @@
     <t>SPRINT</t>
   </si>
   <si>
-    <t>Estimativa</t>
-  </si>
-  <si>
     <t>UC004 - Manter Cotação</t>
   </si>
   <si>
-    <t>UC006 - Emitir aviso de Vencimento</t>
-  </si>
-  <si>
     <t>UC009 - Manter Apólice</t>
   </si>
   <si>
@@ -60,14 +54,20 @@
     <t>UC010 - Gerar renovação apolice</t>
   </si>
   <si>
-    <t>A tecnica de estimativa utilizada foi UCP, devido a facilidade de estimativa do software</t>
+    <t>Estimativa em horas</t>
+  </si>
+  <si>
+    <t>UC006 - Consultar informações</t>
+  </si>
+  <si>
+    <t>A tecnica de estimativa utilizada foi UCP, devido a facilidade de estimativa do software com casos de uso já desenvolvidos;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -325,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -363,6 +371,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,20 +666,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -681,151 +690,172 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="5">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="5">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D10" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1">
       <c r="A11" s="7">
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="8">
         <v>3</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="13" spans="1:4">
+      <c r="D11" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1"/>
+    <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="13"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="13"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -855,7 +885,7 @@
       <c r="C20" s="14"/>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+    <row r="21" spans="1:4" ht="15" thickBot="1">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -876,7 +906,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -888,7 +918,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>